<commit_message>
EPBDS-8671 Automatically detect Map and Collection elements type in test method if method tests a method with collect parameters
</commit_message>
<xml_diff>
--- a/STUDIO/org.openl.rules.test/test-resources/functionality/EPBDS-8671_CollectParametersValidation.xlsx
+++ b/STUDIO/org.openl.rules.test/test-resources/functionality/EPBDS-8671_CollectParametersValidation.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\OPENL\STUDIO\org.openl.rules.test\test-resources\functionality\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58B0200B-D388-4D35-9D9A-FDCECDA30DAA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4425" yWindow="1290" windowWidth="31485" windowHeight="15300"/>
+    <workbookView xWindow="11190" yWindow="135" windowWidth="26505" windowHeight="19350" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="24">
   <si>
     <t>A</t>
   </si>
@@ -58,18 +64,44 @@
     <t xml:space="preserve"> 10+ </t>
   </si>
   <si>
-    <t>SimpleRules  Collect as Inte1ger  and Integer  Map testSimpleRulesMap2 (Integer a, String b)</t>
+    <t>SmartRules  Collect as Double and Double Map testSmartRulesMap1 (Integer a, String b)</t>
+  </si>
+  <si>
+    <t>Test testSmartRulesMap1 testSmartRulesMap1Test</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>_res_["key1"]</t>
+  </si>
+  <si>
+    <t>_res_["key2"]</t>
+  </si>
+  <si>
+    <t>_res_["key3"]</t>
+  </si>
+  <si>
+    <t>_res_["key4"]</t>
+  </si>
+  <si>
+    <t>Result</t>
+  </si>
+  <si>
+    <t>1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
-      <color theme="1" rgb="000000"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -93,7 +125,7 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -102,7 +134,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="2">
     <dxf>
@@ -129,7 +161,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
       <tableStyleElement type="wholeTable" dxfId="1"/>
       <tableStyleElement type="headerRow" dxfId="0"/>
     </tableStyle>
@@ -146,9 +178,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Стандартная">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -186,9 +218,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Стандартная">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -221,9 +253,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -256,9 +305,26 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Стандартная">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -431,18 +497,18 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:F7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="B2:G27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:XFD71"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" customWidth="true" width="20.85546875" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="22.5703125" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="22.7109375" collapsed="true"/>
+    <col min="2" max="2" width="20.85546875" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="22.5703125" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="22.7109375" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:6" x14ac:dyDescent="0.25">
@@ -533,9 +599,166 @@
         <v>3</v>
       </c>
     </row>
+    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B14" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+    </row>
+    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>0</v>
+      </c>
+      <c r="C15" t="s">
+        <v>6</v>
+      </c>
+      <c r="D15" t="s">
+        <v>0</v>
+      </c>
+      <c r="E15" t="s">
+        <v>6</v>
+      </c>
+      <c r="F15" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B16">
+        <v>1</v>
+      </c>
+      <c r="C16" t="s">
+        <v>1</v>
+      </c>
+      <c r="D16">
+        <v>1</v>
+      </c>
+      <c r="F16" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B17">
+        <v>1</v>
+      </c>
+      <c r="C17" t="s">
+        <v>1</v>
+      </c>
+      <c r="D17">
+        <v>2</v>
+      </c>
+      <c r="E17" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B18">
+        <v>2</v>
+      </c>
+      <c r="C18" t="s">
+        <v>2</v>
+      </c>
+      <c r="D18">
+        <v>3</v>
+      </c>
+      <c r="E18" t="s">
+        <v>5</v>
+      </c>
+      <c r="F18" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B19">
+        <v>1</v>
+      </c>
+      <c r="C19" t="s">
+        <v>1</v>
+      </c>
+      <c r="D19">
+        <v>4</v>
+      </c>
+      <c r="E19" t="s">
+        <v>3</v>
+      </c>
+      <c r="F19" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B24" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
+      <c r="G24" s="1"/>
+    </row>
+    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>16</v>
+      </c>
+      <c r="C25" t="s">
+        <v>17</v>
+      </c>
+      <c r="D25" t="s">
+        <v>18</v>
+      </c>
+      <c r="E25" t="s">
+        <v>19</v>
+      </c>
+      <c r="F25" t="s">
+        <v>20</v>
+      </c>
+      <c r="G25" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>0</v>
+      </c>
+      <c r="C26" t="s">
+        <v>6</v>
+      </c>
+      <c r="D26" t="s">
+        <v>22</v>
+      </c>
+      <c r="E26" t="s">
+        <v>22</v>
+      </c>
+      <c r="F26" t="s">
+        <v>22</v>
+      </c>
+      <c r="G26" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>23</v>
+      </c>
+      <c r="C27" t="s">
+        <v>1</v>
+      </c>
+      <c r="D27" t="s">
+        <v>4</v>
+      </c>
+      <c r="E27" t="s">
+        <v>7</v>
+      </c>
+      <c r="G27" t="s">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="3">
     <mergeCell ref="B2:F2"/>
+    <mergeCell ref="B14:F14"/>
+    <mergeCell ref="B24:G24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
EPBDS-10709 Remove usage of SyntaxNodeExceptionCollector.addSyntaxNodeException()
</commit_message>
<xml_diff>
--- a/STUDIO/org.openl.rules.test/test-resources/functionality/EPBDS-8671_CollectParametersValidation.xlsx
+++ b/STUDIO/org.openl.rules.test/test-resources/functionality/EPBDS-8671_CollectParametersValidation.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\OPENL\STUDIO\org.openl.rules.test\test-resources\functionality\"/>
     </mc:Choice>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="43">
   <si>
     <t>A</t>
   </si>
@@ -92,16 +92,74 @@
   </si>
   <si>
     <t>1</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>testX</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>22</t>
+  </si>
+  <si>
+    <t>23</t>
+  </si>
+  <si>
+    <t>24</t>
+  </si>
+  <si>
+    <t>25</t>
+  </si>
+  <si>
+    <t>26</t>
+  </si>
+  <si>
+    <t>27</t>
+  </si>
+  <si>
+    <t>2.2</t>
+  </si>
+  <si>
+    <t>2.6</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
+  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color theme="1" rgb="000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -125,7 +183,7 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -506,9 +564,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="20.85546875" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="22.5703125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="22.7109375" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" customWidth="true" width="20.85546875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="22.5703125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="22.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:6" x14ac:dyDescent="0.25">
@@ -548,7 +606,7 @@
         <v>8</v>
       </c>
       <c r="F4" t="s">
-        <v>4</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.25">
@@ -562,7 +620,7 @@
         <v>9</v>
       </c>
       <c r="E5" t="s">
-        <v>7</v>
+        <v>42</v>
       </c>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.25">
@@ -576,10 +634,10 @@
         <v>10</v>
       </c>
       <c r="E6" t="s">
-        <v>5</v>
+        <v>38</v>
       </c>
       <c r="F6" t="s">
-        <v>5</v>
+        <v>37</v>
       </c>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.25">
@@ -593,11 +651,78 @@
         <v>11</v>
       </c>
       <c r="E7" t="s">
-        <v>3</v>
+        <v>36</v>
       </c>
       <c r="F7" t="s">
-        <v>3</v>
-      </c>
+        <v>41</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="B8" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="E8" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="F8" s="0"/>
+    </row>
+    <row r="9">
+      <c r="B9" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="D9" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="E9" s="0"/>
+      <c r="F9" s="0" t="n">
+        <v>7.0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="B10" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="D10" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="E10" s="0"/>
+      <c r="F10" s="0"/>
+    </row>
+    <row r="11">
+      <c r="B11" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="D11" s="0"/>
+      <c r="E11" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="F11" s="0"/>
+    </row>
+    <row r="12">
+      <c r="B12" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="D12" s="0"/>
+      <c r="E12" s="0"/>
+      <c r="F12" s="0"/>
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">

</xml_diff>